<commit_message>
Missing program 6 description.
</commit_message>
<xml_diff>
--- a/docs/test_programs.xlsx
+++ b/docs/test_programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -144,6 +144,37 @@
         <scheme val="minor"/>
       </rPr>
       <t>ldc.i4.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instruction.</t>
+    </r>
+  </si>
+  <si>
+    <t>write_2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A simple program which pushes 2 on the stack using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ldc.i4.2</t>
     </r>
     <r>
       <rPr>
@@ -532,7 +563,7 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="54" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -610,9 +641,15 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>